<commit_message>
ERS (first working implementation)
</commit_message>
<xml_diff>
--- a/spårväxel_LCC/LCC_Kimstad_maj23(automatiskt återställd).xlsx
+++ b/spårväxel_LCC/LCC_Kimstad_maj23(automatiskt återställd).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdouAA\Work Folders\Documents\GitHub\mistra-inframaint\spårväxel_LCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633DCE94-9F8C-4297-A172-8EE44FAD17EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6538D970-9CCB-45C9-B848-8F3E0DCF2C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-16932" yWindow="1860" windowWidth="17304" windowHeight="9048" tabRatio="807" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="807" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance strategy" sheetId="5" r:id="rId1"/>
@@ -1406,6 +1406,7 @@
     <xf numFmtId="0" fontId="9" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="9" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1415,7 +1416,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bra" xfId="2" builtinId="26"/>
@@ -8706,7 +8706,7 @@
       <c r="F3" s="2">
         <v>2</v>
       </c>
-      <c r="G3" s="139" t="s">
+      <c r="G3" s="140" t="s">
         <v>28</v>
       </c>
       <c r="I3" s="10" t="s">
@@ -8741,7 +8741,7 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="140"/>
+      <c r="G4" s="141"/>
       <c r="I4" s="20">
         <v>41778.839583333298</v>
       </c>
@@ -8777,7 +8777,7 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="140"/>
+      <c r="G5" s="141"/>
       <c r="I5" s="20">
         <v>41865.585416666698</v>
       </c>
@@ -8808,7 +8808,7 @@
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6" s="140"/>
+      <c r="G6" s="141"/>
       <c r="I6" s="23">
         <v>41883</v>
       </c>
@@ -8839,7 +8839,7 @@
       <c r="F7" s="5">
         <v>2</v>
       </c>
-      <c r="G7" s="141"/>
+      <c r="G7" s="142"/>
       <c r="I7" s="24">
         <v>41913</v>
       </c>
@@ -9001,7 +9001,7 @@
       <c r="F17" s="132">
         <v>1</v>
       </c>
-      <c r="G17" s="139" t="s">
+      <c r="G17" s="140" t="s">
         <v>28</v>
       </c>
       <c r="I17" s="17">
@@ -9034,7 +9034,7 @@
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="G18" s="140"/>
+      <c r="G18" s="141"/>
       <c r="I18" s="15">
         <v>42475</v>
       </c>
@@ -9065,7 +9065,7 @@
       <c r="F19">
         <v>0</v>
       </c>
-      <c r="G19" s="140"/>
+      <c r="G19" s="141"/>
       <c r="I19" s="16">
         <v>42475</v>
       </c>
@@ -9096,7 +9096,7 @@
       <c r="F20">
         <v>0</v>
       </c>
-      <c r="G20" s="140"/>
+      <c r="G20" s="141"/>
       <c r="I20" s="18">
         <v>42487</v>
       </c>
@@ -9127,7 +9127,7 @@
       <c r="F21" s="5">
         <v>0</v>
       </c>
-      <c r="G21" s="141"/>
+      <c r="G21" s="142"/>
       <c r="I21" s="19">
         <v>42491</v>
       </c>
@@ -10097,7 +10097,7 @@
       <c r="G50" t="s">
         <v>48</v>
       </c>
-      <c r="I50" s="142" t="s">
+      <c r="I50" s="139" t="s">
         <v>222</v>
       </c>
     </row>

</xml_diff>